<commit_message>
Aquatic terrestrial IDs updated, figures updated, new questions added
Added Danielle's insect ID files and created a new unique_families_aquatic_terrestrial_IDs.csv file. Changed sizes of figures. Added a few more questions/starts of figures.
</commit_message>
<xml_diff>
--- a/5_other_outputs/unique_families_aquatic_terrestrial_IDs_tjl.xlsx
+++ b/5_other_outputs/unique_families_aquatic_terrestrial_IDs_tjl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juehling/Dropbox/tres_coi_analysis_2019/5_other_outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2972C2BB-2CDF-4C0A-82F9-CE81890CC403}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B7FE01-CC1C-D748-A0CF-7167828DC115}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30420" yWindow="-320" windowWidth="29200" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unique_families_aquatic_terrest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="772">
   <si>
     <t>order_for_organization</t>
   </si>
@@ -1924,6 +1924,441 @@
   </si>
   <si>
     <t>likely terrestrial</t>
+  </si>
+  <si>
+    <t>Acanthosomatidae</t>
+  </si>
+  <si>
+    <t>Shield bugs</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/14006</t>
+  </si>
+  <si>
+    <t>Adelidae</t>
+  </si>
+  <si>
+    <t>Fairy moths</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/34115</t>
+  </si>
+  <si>
+    <t>Ameletidae</t>
+  </si>
+  <si>
+    <t>Combmouthed Minnow Mayflies</t>
+  </si>
+  <si>
+    <t>https://www.naturebob.com/sites/default/files/Mayflies%20by%20John%20Hudson,%20Katherine%20Hocker,%20Robert%20H.%20Armstrong.pdf</t>
+  </si>
+  <si>
+    <t>Amphipsocidae</t>
+  </si>
+  <si>
+    <t>appears to be only one species in NA, terrestrial</t>
+  </si>
+  <si>
+    <t>Hairy-winged Barklice</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Psocoptera</t>
+  </si>
+  <si>
+    <t>Lay eggs in foliage, and are found on bark. But also sometimes eat algae?</t>
+  </si>
+  <si>
+    <t>Berytidae</t>
+  </si>
+  <si>
+    <t>Stilt Bugs</t>
+  </si>
+  <si>
+    <t>https://www.britannica.com/animal/stilt-bug</t>
+  </si>
+  <si>
+    <t>Found in home gardens and feeding on crops</t>
+  </si>
+  <si>
+    <t>Buprestidae</t>
+  </si>
+  <si>
+    <t>Metallic Wood-boring Beetles</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Buprestidae</t>
+  </si>
+  <si>
+    <t>Cerambycidae</t>
+  </si>
+  <si>
+    <t>Long-horned beetles</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Longhorn_beetle</t>
+  </si>
+  <si>
+    <t>Cleridae</t>
+  </si>
+  <si>
+    <t>Checkered beetles</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Cleridae</t>
+  </si>
+  <si>
+    <t>Clubionidae</t>
+  </si>
+  <si>
+    <t>Sac spiders</t>
+  </si>
+  <si>
+    <t>http://www.bio.brandeis.edu/fieldbio/Spiders_Savransky_Suhd_Brondstatter/Pages/Fam_Clubionidae.html</t>
+  </si>
+  <si>
+    <t>Coccinellidae</t>
+  </si>
+  <si>
+    <t>Lady bug</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Coccinellidae</t>
+  </si>
+  <si>
+    <t>Conopidae</t>
+  </si>
+  <si>
+    <t>Thick-headed flies</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/92</t>
+  </si>
+  <si>
+    <t>Cosmopterigidae</t>
+  </si>
+  <si>
+    <t>Cosmet moths</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/21341</t>
+  </si>
+  <si>
+    <t>Derbidae</t>
+  </si>
+  <si>
+    <t>Derbid Planthoppers</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Derbidae</t>
+  </si>
+  <si>
+    <t>Diprionidae</t>
+  </si>
+  <si>
+    <t>Conifer sawflies</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Diprionidae</t>
+  </si>
+  <si>
+    <t>Entomobryomorpha</t>
+  </si>
+  <si>
+    <t>Entomobryidae</t>
+  </si>
+  <si>
+    <t>Slender Springtails</t>
+  </si>
+  <si>
+    <t>https://www-sciencedirect-com.proxy.library.cornell.edu/topics/agricultural-and-biological-sciences/entomobryidae</t>
+  </si>
+  <si>
+    <t>Eucnemidae</t>
+  </si>
+  <si>
+    <t>False Click beetles</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/63946</t>
+  </si>
+  <si>
+    <t>Helicopsychidae</t>
+  </si>
+  <si>
+    <t>Snail-cased caddisflies</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/52437</t>
+  </si>
+  <si>
+    <t>Hydroptilidae</t>
+  </si>
+  <si>
+    <t>Microcaddisflies</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/118384</t>
+  </si>
+  <si>
+    <t>Hydryphantidae</t>
+  </si>
+  <si>
+    <t>https://www.biotaxa.org/saa/article/view/saa.19.2.6</t>
+  </si>
+  <si>
+    <t>Isotomidae</t>
+  </si>
+  <si>
+    <t>Collembola are mostly soil-dwellers</t>
+  </si>
+  <si>
+    <t>https://zookeys.pensoft.net/article/49363/</t>
+  </si>
+  <si>
+    <t>This seems to be a fairly new family and there is almost no information on it. There is no common name either</t>
+  </si>
+  <si>
+    <t>Latridiidae</t>
+  </si>
+  <si>
+    <t>Minute brown Scavenger beetles</t>
+  </si>
+  <si>
+    <t>https://www.mindat.org/taxon-7834.html</t>
+  </si>
+  <si>
+    <t>Lygaeidae</t>
+  </si>
+  <si>
+    <t>Seed bugs</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/129</t>
+  </si>
+  <si>
+    <t>Macronyssidae</t>
+  </si>
+  <si>
+    <t>https://www-sciencedirect-com.proxy.library.cornell.edu/topics/agricultural-and-biological-sciences/macronyssidae</t>
+  </si>
+  <si>
+    <t>parasitic mites</t>
+  </si>
+  <si>
+    <t>Megaspilidae</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/155554</t>
+  </si>
+  <si>
+    <t>parasites</t>
+  </si>
+  <si>
+    <t>Micropezidae</t>
+  </si>
+  <si>
+    <t>Stilt-legged Flies</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/134</t>
+  </si>
+  <si>
+    <t>found in moist environments, but eat rotting fruit. Unsure on classification</t>
+  </si>
+  <si>
+    <t>Mimetidae</t>
+  </si>
+  <si>
+    <t>Pirate spiders</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Pirate_spider</t>
+  </si>
+  <si>
+    <t>Odontoceridae</t>
+  </si>
+  <si>
+    <t>Mortarjoint Casemaker Caddisflies</t>
+  </si>
+  <si>
+    <t>https://seetolearn.weebly.com/uploads/4/6/7/4/46744079/trichoptera_order_sheet.pdf</t>
+  </si>
+  <si>
+    <t>Oestridae</t>
+  </si>
+  <si>
+    <t>Bot flies</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Botfly</t>
+  </si>
+  <si>
+    <t>Pachygronthidae</t>
+  </si>
+  <si>
+    <t>https://www.americaninsects.net/ht/pachygronthidae.html</t>
+  </si>
+  <si>
+    <t>I think they are also seed bugs?</t>
+  </si>
+  <si>
+    <t>Perilampidae</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/16771</t>
+  </si>
+  <si>
+    <t>Psenidae</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Psenini</t>
+  </si>
+  <si>
+    <t>Parasitic wasps; classification is questioned in literature. I am guessing terrestrial</t>
+  </si>
+  <si>
+    <t>Psychomyiidae</t>
+  </si>
+  <si>
+    <t>Net Tube Caddisflies</t>
+  </si>
+  <si>
+    <t>Pyrochroidae</t>
+  </si>
+  <si>
+    <t>Fire-Colored beetles</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/9123</t>
+  </si>
+  <si>
+    <t>Blattodea</t>
+  </si>
+  <si>
+    <t>Rhinotermitidae</t>
+  </si>
+  <si>
+    <t>Subterranean termites</t>
+  </si>
+  <si>
+    <t>Rhyparochromidae</t>
+  </si>
+  <si>
+    <t>Dirt-colored seed bugs</t>
+  </si>
+  <si>
+    <t>http://www.arizonensis.org/sonoran/fieldguide/arthropoda/rhyparochromidae.html#:~:text=Seed%20bugs%20as%20their%20name,beneath%20rocks%20or%20leaf%20litter.</t>
+  </si>
+  <si>
+    <t>Scraptiidae</t>
+  </si>
+  <si>
+    <t>False Flower Beetles</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/51373</t>
+  </si>
+  <si>
+    <t>Scutacaridae</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/258227720_Mites_of_the_family_Scutacaridae_of_Eastern_Palaearctic</t>
+  </si>
+  <si>
+    <t>mites</t>
+  </si>
+  <si>
+    <t>Scutelleridae</t>
+  </si>
+  <si>
+    <t>Shield-backed Bugs</t>
+  </si>
+  <si>
+    <t>https://www.merriam-webster.com/dictionary/Scutelleridae</t>
+  </si>
+  <si>
+    <t>Tenebrionidae</t>
+  </si>
+  <si>
+    <t>Darkling beetles</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/152</t>
+  </si>
+  <si>
+    <t>Tetragnathidae</t>
+  </si>
+  <si>
+    <t>Long-jawed orb weavers</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/1958</t>
+  </si>
+  <si>
+    <t>Orthoptera</t>
+  </si>
+  <si>
+    <t>Tetrigidae</t>
+  </si>
+  <si>
+    <t>terrestrial, eggs sometimes laid underwater but the nymphs don't stay there</t>
+  </si>
+  <si>
+    <t>Pygmy grasshoppers</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/106</t>
+  </si>
+  <si>
+    <t>could be just aquatic. Not positive</t>
+  </si>
+  <si>
+    <t>Theridiidae</t>
+  </si>
+  <si>
+    <t>Cobweb Spiders</t>
+  </si>
+  <si>
+    <t>http://www.biokids.umich.edu/critters/Theridiidae/#:~:text=These%20spiders%20live%20in%20many,group%20are%20common%20house%20spiders.</t>
+  </si>
+  <si>
+    <t>Thyreocoridae</t>
+  </si>
+  <si>
+    <t>Ebony bugs</t>
+  </si>
+  <si>
+    <t>https://bugguide.net/node/view/6985</t>
+  </si>
+  <si>
+    <t>Torrenticolidae</t>
+  </si>
+  <si>
+    <t>Torrent mites</t>
+  </si>
+  <si>
+    <t>https://www.biotaxa.org/Zootaxa/article/view/zootaxa.3840.1.1/0</t>
+  </si>
+  <si>
+    <t>Could be both.</t>
+  </si>
+  <si>
+    <t>Isopoda</t>
+  </si>
+  <si>
+    <t>Trachelipodidae</t>
+  </si>
+  <si>
+    <t>Wood mites</t>
+  </si>
+  <si>
+    <t>http://www.marinespecies.org/aphia.php?p=taxdetails&amp;id=248325</t>
+  </si>
+  <si>
+    <t>Tydeidae</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/325107107_Tydeinae_mites_Acariformes_Prostigmata_Tydeidae_from_bird_nests_with_description_of_three_new_species</t>
   </si>
 </sst>
 </file>
@@ -2772,24 +3207,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H169"/>
+  <dimension ref="A1:H215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="A1:H215"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2815,7 +3251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2841,7 +3277,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2867,7 +3303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2893,7 +3329,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2916,7 +3352,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2939,7 +3375,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2965,7 +3401,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2982,7 +3418,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2999,7 +3435,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -3025,7 +3461,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -3051,7 +3487,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -3068,7 +3504,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -3085,7 +3521,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -3102,7 +3538,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -3128,7 +3564,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -3145,7 +3581,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -3162,7 +3598,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -3179,7 +3615,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -3205,7 +3641,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -3228,7 +3664,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -3245,7 +3681,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -3262,7 +3698,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -3279,7 +3715,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -3302,7 +3738,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -3325,7 +3761,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -3345,7 +3781,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -3371,7 +3807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -3388,7 +3824,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -3414,7 +3850,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -3440,7 +3876,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>104</v>
       </c>
@@ -3466,7 +3902,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -3483,7 +3919,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>104</v>
       </c>
@@ -3509,7 +3945,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>104</v>
       </c>
@@ -3529,7 +3965,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>104</v>
       </c>
@@ -3549,7 +3985,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -3566,7 +4002,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>104</v>
       </c>
@@ -3592,7 +4028,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>104</v>
       </c>
@@ -3618,7 +4054,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>104</v>
       </c>
@@ -3635,7 +4071,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>104</v>
       </c>
@@ -3661,7 +4097,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>104</v>
       </c>
@@ -3681,7 +4117,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>104</v>
       </c>
@@ -3698,7 +4134,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>104</v>
       </c>
@@ -3724,7 +4160,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>104</v>
       </c>
@@ -3741,7 +4177,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -3764,7 +4200,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>104</v>
       </c>
@@ -3781,7 +4217,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -3798,7 +4234,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>104</v>
       </c>
@@ -3815,7 +4251,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -3832,7 +4268,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>104</v>
       </c>
@@ -3849,7 +4285,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>104</v>
       </c>
@@ -3869,7 +4305,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -3889,7 +4325,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -3915,7 +4351,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -3941,7 +4377,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>104</v>
       </c>
@@ -3961,7 +4397,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -3978,7 +4414,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>104</v>
       </c>
@@ -4004,7 +4440,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -4027,7 +4463,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>104</v>
       </c>
@@ -4047,7 +4483,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>104</v>
       </c>
@@ -4064,7 +4500,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>104</v>
       </c>
@@ -4081,7 +4517,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>104</v>
       </c>
@@ -4098,7 +4534,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>104</v>
       </c>
@@ -4124,7 +4560,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>104</v>
       </c>
@@ -4150,7 +4586,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>104</v>
       </c>
@@ -4173,7 +4609,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>104</v>
       </c>
@@ -4199,7 +4635,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>104</v>
       </c>
@@ -4216,7 +4652,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>104</v>
       </c>
@@ -4233,7 +4669,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>104</v>
       </c>
@@ -4250,7 +4686,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>104</v>
       </c>
@@ -4270,7 +4706,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>104</v>
       </c>
@@ -4293,7 +4729,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>104</v>
       </c>
@@ -4313,7 +4749,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>104</v>
       </c>
@@ -4330,7 +4766,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>104</v>
       </c>
@@ -4347,7 +4783,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>104</v>
       </c>
@@ -4364,7 +4800,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>104</v>
       </c>
@@ -4381,7 +4817,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>104</v>
       </c>
@@ -4404,7 +4840,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>104</v>
       </c>
@@ -4421,7 +4857,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>104</v>
       </c>
@@ -4447,7 +4883,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>104</v>
       </c>
@@ -4464,7 +4900,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>104</v>
       </c>
@@ -4487,7 +4923,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>104</v>
       </c>
@@ -4513,7 +4949,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>104</v>
       </c>
@@ -4539,7 +4975,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>299</v>
       </c>
@@ -4556,7 +4992,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>299</v>
       </c>
@@ -4573,7 +5009,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>299</v>
       </c>
@@ -4590,7 +5026,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>299</v>
       </c>
@@ -4610,7 +5046,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>299</v>
       </c>
@@ -4636,7 +5072,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>299</v>
       </c>
@@ -4653,7 +5089,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>299</v>
       </c>
@@ -4670,7 +5106,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>299</v>
       </c>
@@ -4687,7 +5123,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>299</v>
       </c>
@@ -4704,7 +5140,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>329</v>
       </c>
@@ -4721,7 +5157,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>329</v>
       </c>
@@ -4747,7 +5183,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>329</v>
       </c>
@@ -4773,7 +5209,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>329</v>
       </c>
@@ -4793,7 +5229,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>329</v>
       </c>
@@ -4810,7 +5246,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>329</v>
       </c>
@@ -4827,7 +5263,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>329</v>
       </c>
@@ -4850,7 +5286,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>329</v>
       </c>
@@ -4867,7 +5303,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>329</v>
       </c>
@@ -4887,7 +5323,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>329</v>
       </c>
@@ -4907,7 +5343,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>329</v>
       </c>
@@ -4930,7 +5366,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>368</v>
       </c>
@@ -4953,7 +5389,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>368</v>
       </c>
@@ -4970,7 +5406,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>368</v>
       </c>
@@ -4990,7 +5426,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>368</v>
       </c>
@@ -5007,7 +5443,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>368</v>
       </c>
@@ -5027,7 +5463,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>368</v>
       </c>
@@ -5053,7 +5489,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>368</v>
       </c>
@@ -5070,7 +5506,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>368</v>
       </c>
@@ -5087,7 +5523,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>368</v>
       </c>
@@ -5104,7 +5540,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>398</v>
       </c>
@@ -5130,7 +5566,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>398</v>
       </c>
@@ -5156,7 +5592,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>398</v>
       </c>
@@ -5182,7 +5618,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>398</v>
       </c>
@@ -5199,7 +5635,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>398</v>
       </c>
@@ -5216,7 +5652,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>398</v>
       </c>
@@ -5233,7 +5669,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>398</v>
       </c>
@@ -5250,7 +5686,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>398</v>
       </c>
@@ -5267,7 +5703,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>398</v>
       </c>
@@ -5284,7 +5720,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>398</v>
       </c>
@@ -5301,7 +5737,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>398</v>
       </c>
@@ -5318,7 +5754,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>398</v>
       </c>
@@ -5335,7 +5771,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>398</v>
       </c>
@@ -5352,7 +5788,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>398</v>
       </c>
@@ -5369,7 +5805,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>398</v>
       </c>
@@ -5386,7 +5822,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>447</v>
       </c>
@@ -5403,7 +5839,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>451</v>
       </c>
@@ -5429,7 +5865,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>451</v>
       </c>
@@ -5455,7 +5891,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>451</v>
       </c>
@@ -5472,7 +5908,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>451</v>
       </c>
@@ -5495,7 +5931,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>465</v>
       </c>
@@ -5518,7 +5954,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>469</v>
       </c>
@@ -5535,7 +5971,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>469</v>
       </c>
@@ -5549,7 +5985,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>469</v>
       </c>
@@ -5566,7 +6002,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>469</v>
       </c>
@@ -5592,7 +6028,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>469</v>
       </c>
@@ -5609,7 +6045,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>469</v>
       </c>
@@ -5626,7 +6062,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>488</v>
       </c>
@@ -5646,7 +6082,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>488</v>
       </c>
@@ -5663,7 +6099,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>488</v>
       </c>
@@ -5689,7 +6125,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>488</v>
       </c>
@@ -5706,7 +6142,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>488</v>
       </c>
@@ -5723,7 +6159,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>506</v>
       </c>
@@ -5749,7 +6185,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>511</v>
       </c>
@@ -5775,7 +6211,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>511</v>
       </c>
@@ -5801,7 +6237,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>511</v>
       </c>
@@ -5824,7 +6260,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>511</v>
       </c>
@@ -5847,7 +6283,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>511</v>
       </c>
@@ -5870,7 +6306,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>529</v>
       </c>
@@ -5896,7 +6332,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>534</v>
       </c>
@@ -5916,7 +6352,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>537</v>
       </c>
@@ -5933,7 +6369,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>537</v>
       </c>
@@ -5950,7 +6386,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>537</v>
       </c>
@@ -5967,7 +6403,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>537</v>
       </c>
@@ -5984,7 +6420,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>537</v>
       </c>
@@ -6001,7 +6437,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>537</v>
       </c>
@@ -6018,7 +6454,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>537</v>
       </c>
@@ -6035,7 +6471,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>559</v>
       </c>
@@ -6061,7 +6497,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>559</v>
       </c>
@@ -6084,7 +6520,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>559</v>
       </c>
@@ -6107,7 +6543,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>559</v>
       </c>
@@ -6127,7 +6563,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>559</v>
       </c>
@@ -6150,7 +6586,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>559</v>
       </c>
@@ -6176,7 +6612,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>559</v>
       </c>
@@ -6199,7 +6635,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>559</v>
       </c>
@@ -6222,7 +6658,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>559</v>
       </c>
@@ -6248,7 +6684,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>610</v>
       </c>
@@ -6263,6 +6699,860 @@
       </c>
       <c r="H169" t="s">
         <v>589</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>329</v>
+      </c>
+      <c r="B170" t="s">
+        <v>627</v>
+      </c>
+      <c r="C170" t="s">
+        <v>9</v>
+      </c>
+      <c r="F170" t="s">
+        <v>628</v>
+      </c>
+      <c r="G170" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>398</v>
+      </c>
+      <c r="B171" t="s">
+        <v>630</v>
+      </c>
+      <c r="C171" t="s">
+        <v>9</v>
+      </c>
+      <c r="F171" t="s">
+        <v>631</v>
+      </c>
+      <c r="G171" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>299</v>
+      </c>
+      <c r="B172" t="s">
+        <v>633</v>
+      </c>
+      <c r="C172" t="s">
+        <v>48</v>
+      </c>
+      <c r="F172" t="s">
+        <v>634</v>
+      </c>
+      <c r="G172" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>506</v>
+      </c>
+      <c r="B173" t="s">
+        <v>636</v>
+      </c>
+      <c r="C173" t="s">
+        <v>9</v>
+      </c>
+      <c r="D173" t="s">
+        <v>10</v>
+      </c>
+      <c r="E173" t="s">
+        <v>637</v>
+      </c>
+      <c r="F173" t="s">
+        <v>638</v>
+      </c>
+      <c r="G173" t="s">
+        <v>639</v>
+      </c>
+      <c r="H173" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>329</v>
+      </c>
+      <c r="B174" t="s">
+        <v>641</v>
+      </c>
+      <c r="C174" t="s">
+        <v>9</v>
+      </c>
+      <c r="F174" t="s">
+        <v>642</v>
+      </c>
+      <c r="G174" t="s">
+        <v>643</v>
+      </c>
+      <c r="H174" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>38</v>
+      </c>
+      <c r="B175" t="s">
+        <v>645</v>
+      </c>
+      <c r="C175" t="s">
+        <v>9</v>
+      </c>
+      <c r="F175" t="s">
+        <v>646</v>
+      </c>
+      <c r="G175" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>38</v>
+      </c>
+      <c r="B176" t="s">
+        <v>648</v>
+      </c>
+      <c r="C176" t="s">
+        <v>9</v>
+      </c>
+      <c r="F176" t="s">
+        <v>649</v>
+      </c>
+      <c r="G176" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>38</v>
+      </c>
+      <c r="B177" t="s">
+        <v>651</v>
+      </c>
+      <c r="C177" t="s">
+        <v>9</v>
+      </c>
+      <c r="F177" t="s">
+        <v>652</v>
+      </c>
+      <c r="G177" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>7</v>
+      </c>
+      <c r="B178" t="s">
+        <v>654</v>
+      </c>
+      <c r="C178" t="s">
+        <v>9</v>
+      </c>
+      <c r="F178" t="s">
+        <v>655</v>
+      </c>
+      <c r="G178" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>38</v>
+      </c>
+      <c r="B179" t="s">
+        <v>657</v>
+      </c>
+      <c r="C179" t="s">
+        <v>9</v>
+      </c>
+      <c r="F179" t="s">
+        <v>658</v>
+      </c>
+      <c r="G179" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>104</v>
+      </c>
+      <c r="B180" t="s">
+        <v>660</v>
+      </c>
+      <c r="C180" t="s">
+        <v>9</v>
+      </c>
+      <c r="F180" t="s">
+        <v>661</v>
+      </c>
+      <c r="G180" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>398</v>
+      </c>
+      <c r="B181" t="s">
+        <v>663</v>
+      </c>
+      <c r="C181" t="s">
+        <v>9</v>
+      </c>
+      <c r="F181" t="s">
+        <v>664</v>
+      </c>
+      <c r="G181" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>329</v>
+      </c>
+      <c r="B182" t="s">
+        <v>666</v>
+      </c>
+      <c r="C182" t="s">
+        <v>9</v>
+      </c>
+      <c r="F182" t="s">
+        <v>667</v>
+      </c>
+      <c r="G182" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>368</v>
+      </c>
+      <c r="B183" t="s">
+        <v>669</v>
+      </c>
+      <c r="C183" t="s">
+        <v>9</v>
+      </c>
+      <c r="F183" t="s">
+        <v>670</v>
+      </c>
+      <c r="G183" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>672</v>
+      </c>
+      <c r="B184" t="s">
+        <v>673</v>
+      </c>
+      <c r="C184" t="s">
+        <v>9</v>
+      </c>
+      <c r="F184" t="s">
+        <v>674</v>
+      </c>
+      <c r="G184" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>38</v>
+      </c>
+      <c r="B185" t="s">
+        <v>676</v>
+      </c>
+      <c r="C185" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" t="s">
+        <v>677</v>
+      </c>
+      <c r="G185" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>537</v>
+      </c>
+      <c r="B186" t="s">
+        <v>679</v>
+      </c>
+      <c r="C186" t="s">
+        <v>48</v>
+      </c>
+      <c r="F186" t="s">
+        <v>680</v>
+      </c>
+      <c r="G186" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>537</v>
+      </c>
+      <c r="B187" t="s">
+        <v>682</v>
+      </c>
+      <c r="C187" t="s">
+        <v>48</v>
+      </c>
+      <c r="F187" t="s">
+        <v>683</v>
+      </c>
+      <c r="G187" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>559</v>
+      </c>
+      <c r="B188" t="s">
+        <v>685</v>
+      </c>
+      <c r="C188" t="s">
+        <v>48</v>
+      </c>
+      <c r="F188" t="s">
+        <v>561</v>
+      </c>
+      <c r="G188" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>93</v>
+      </c>
+      <c r="B189" t="s">
+        <v>687</v>
+      </c>
+      <c r="C189" t="s">
+        <v>48</v>
+      </c>
+      <c r="D189" t="s">
+        <v>10</v>
+      </c>
+      <c r="E189" t="s">
+        <v>688</v>
+      </c>
+      <c r="G189" t="s">
+        <v>689</v>
+      </c>
+      <c r="H189" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>38</v>
+      </c>
+      <c r="B190" t="s">
+        <v>691</v>
+      </c>
+      <c r="C190" t="s">
+        <v>9</v>
+      </c>
+      <c r="F190" t="s">
+        <v>692</v>
+      </c>
+      <c r="G190" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>329</v>
+      </c>
+      <c r="B191" t="s">
+        <v>694</v>
+      </c>
+      <c r="C191" t="s">
+        <v>9</v>
+      </c>
+      <c r="F191" t="s">
+        <v>695</v>
+      </c>
+      <c r="G191" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>451</v>
+      </c>
+      <c r="B192" t="s">
+        <v>697</v>
+      </c>
+      <c r="C192" t="s">
+        <v>9</v>
+      </c>
+      <c r="D192" t="s">
+        <v>10</v>
+      </c>
+      <c r="E192" t="s">
+        <v>9</v>
+      </c>
+      <c r="G192" t="s">
+        <v>698</v>
+      </c>
+      <c r="H192" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>368</v>
+      </c>
+      <c r="B193" t="s">
+        <v>700</v>
+      </c>
+      <c r="C193" t="s">
+        <v>9</v>
+      </c>
+      <c r="D193" t="s">
+        <v>10</v>
+      </c>
+      <c r="E193" t="s">
+        <v>9</v>
+      </c>
+      <c r="G193" t="s">
+        <v>701</v>
+      </c>
+      <c r="H193" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>104</v>
+      </c>
+      <c r="B194" t="s">
+        <v>703</v>
+      </c>
+      <c r="C194" t="s">
+        <v>58</v>
+      </c>
+      <c r="D194" t="s">
+        <v>10</v>
+      </c>
+      <c r="E194" t="s">
+        <v>626</v>
+      </c>
+      <c r="F194" t="s">
+        <v>704</v>
+      </c>
+      <c r="G194" t="s">
+        <v>705</v>
+      </c>
+      <c r="H194" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>7</v>
+      </c>
+      <c r="B195" t="s">
+        <v>707</v>
+      </c>
+      <c r="C195" t="s">
+        <v>9</v>
+      </c>
+      <c r="F195" t="s">
+        <v>708</v>
+      </c>
+      <c r="G195" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>537</v>
+      </c>
+      <c r="B196" t="s">
+        <v>710</v>
+      </c>
+      <c r="C196" t="s">
+        <v>48</v>
+      </c>
+      <c r="F196" t="s">
+        <v>711</v>
+      </c>
+      <c r="G196" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>104</v>
+      </c>
+      <c r="B197" t="s">
+        <v>713</v>
+      </c>
+      <c r="C197" t="s">
+        <v>9</v>
+      </c>
+      <c r="F197" t="s">
+        <v>714</v>
+      </c>
+      <c r="G197" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>329</v>
+      </c>
+      <c r="B198" t="s">
+        <v>716</v>
+      </c>
+      <c r="C198" t="s">
+        <v>9</v>
+      </c>
+      <c r="D198" t="s">
+        <v>10</v>
+      </c>
+      <c r="E198" t="s">
+        <v>626</v>
+      </c>
+      <c r="G198" t="s">
+        <v>717</v>
+      </c>
+      <c r="H198" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>368</v>
+      </c>
+      <c r="B199" t="s">
+        <v>719</v>
+      </c>
+      <c r="C199" t="s">
+        <v>9</v>
+      </c>
+      <c r="G199" t="s">
+        <v>720</v>
+      </c>
+      <c r="H199" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>368</v>
+      </c>
+      <c r="B200" t="s">
+        <v>721</v>
+      </c>
+      <c r="C200" t="s">
+        <v>95</v>
+      </c>
+      <c r="D200" t="s">
+        <v>10</v>
+      </c>
+      <c r="E200" t="s">
+        <v>9</v>
+      </c>
+      <c r="G200" t="s">
+        <v>722</v>
+      </c>
+      <c r="H200" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>537</v>
+      </c>
+      <c r="B201" t="s">
+        <v>724</v>
+      </c>
+      <c r="C201" t="s">
+        <v>48</v>
+      </c>
+      <c r="F201" t="s">
+        <v>725</v>
+      </c>
+      <c r="G201" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>38</v>
+      </c>
+      <c r="B202" t="s">
+        <v>726</v>
+      </c>
+      <c r="C202" t="s">
+        <v>9</v>
+      </c>
+      <c r="F202" t="s">
+        <v>727</v>
+      </c>
+      <c r="G202" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>729</v>
+      </c>
+      <c r="B203" t="s">
+        <v>730</v>
+      </c>
+      <c r="C203" t="s">
+        <v>9</v>
+      </c>
+      <c r="F203" t="s">
+        <v>731</v>
+      </c>
+      <c r="G203" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>329</v>
+      </c>
+      <c r="B204" t="s">
+        <v>732</v>
+      </c>
+      <c r="C204" t="s">
+        <v>9</v>
+      </c>
+      <c r="F204" t="s">
+        <v>733</v>
+      </c>
+      <c r="G204" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>38</v>
+      </c>
+      <c r="B205" t="s">
+        <v>735</v>
+      </c>
+      <c r="C205" t="s">
+        <v>9</v>
+      </c>
+      <c r="F205" t="s">
+        <v>736</v>
+      </c>
+      <c r="G205" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>559</v>
+      </c>
+      <c r="B206" t="s">
+        <v>738</v>
+      </c>
+      <c r="C206" t="s">
+        <v>9</v>
+      </c>
+      <c r="G206" t="s">
+        <v>739</v>
+      </c>
+      <c r="H206" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>329</v>
+      </c>
+      <c r="B207" t="s">
+        <v>741</v>
+      </c>
+      <c r="C207" t="s">
+        <v>9</v>
+      </c>
+      <c r="F207" t="s">
+        <v>742</v>
+      </c>
+      <c r="G207" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>38</v>
+      </c>
+      <c r="B208" t="s">
+        <v>744</v>
+      </c>
+      <c r="C208" t="s">
+        <v>9</v>
+      </c>
+      <c r="F208" t="s">
+        <v>745</v>
+      </c>
+      <c r="G208" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>7</v>
+      </c>
+      <c r="B209" t="s">
+        <v>747</v>
+      </c>
+      <c r="C209" t="s">
+        <v>9</v>
+      </c>
+      <c r="F209" t="s">
+        <v>748</v>
+      </c>
+      <c r="G209" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>750</v>
+      </c>
+      <c r="B210" t="s">
+        <v>751</v>
+      </c>
+      <c r="C210" t="s">
+        <v>58</v>
+      </c>
+      <c r="D210" t="s">
+        <v>10</v>
+      </c>
+      <c r="E210" t="s">
+        <v>752</v>
+      </c>
+      <c r="F210" t="s">
+        <v>753</v>
+      </c>
+      <c r="G210" t="s">
+        <v>754</v>
+      </c>
+      <c r="H210" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>7</v>
+      </c>
+      <c r="B211" t="s">
+        <v>756</v>
+      </c>
+      <c r="C211" t="s">
+        <v>9</v>
+      </c>
+      <c r="F211" t="s">
+        <v>757</v>
+      </c>
+      <c r="G211" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>329</v>
+      </c>
+      <c r="B212" t="s">
+        <v>759</v>
+      </c>
+      <c r="C212" t="s">
+        <v>9</v>
+      </c>
+      <c r="F212" t="s">
+        <v>760</v>
+      </c>
+      <c r="G212" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>559</v>
+      </c>
+      <c r="B213" t="s">
+        <v>762</v>
+      </c>
+      <c r="C213" t="s">
+        <v>48</v>
+      </c>
+      <c r="D213" t="s">
+        <v>10</v>
+      </c>
+      <c r="E213" t="s">
+        <v>48</v>
+      </c>
+      <c r="F213" t="s">
+        <v>763</v>
+      </c>
+      <c r="G213" t="s">
+        <v>764</v>
+      </c>
+      <c r="H213" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>766</v>
+      </c>
+      <c r="B214" t="s">
+        <v>767</v>
+      </c>
+      <c r="C214" t="s">
+        <v>9</v>
+      </c>
+      <c r="F214" t="s">
+        <v>768</v>
+      </c>
+      <c r="G214" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>559</v>
+      </c>
+      <c r="B215" t="s">
+        <v>770</v>
+      </c>
+      <c r="C215" t="s">
+        <v>9</v>
+      </c>
+      <c r="D215" t="s">
+        <v>10</v>
+      </c>
+      <c r="E215" t="s">
+        <v>9</v>
+      </c>
+      <c r="G215" t="s">
+        <v>771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>